<commit_message>
método para criar cabeçalho
</commit_message>
<xml_diff>
--- a/exemplo.xlsx
+++ b/exemplo.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -421,8 +421,23 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+    </row>
     <row r="2">
       <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
         <v>2</v>
       </c>
     </row>

</xml_diff>